<commit_message>
PUNTO 5 Y 6
</commit_message>
<xml_diff>
--- a/programacion2-2025/05-trabajoPractico-Arboles/PUNTO 5 Y 6/TP_5_Arboles_PUNTO_6_ArbolB+.xlsx
+++ b/programacion2-2025/05-trabajoPractico-Arboles/PUNTO 5 Y 6/TP_5_Arboles_PUNTO_6_ArbolB+.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matyx\Desktop\Unlu\Cuatri 3\Prog 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matyx\Desktop\Unlu\Cuatri 3\Prog 2\grupo3renzobisso\programacion2-2025\05-trabajoPractico-Arboles\PUNTO 5 Y 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078F9761-8A9A-43CC-AED1-CB21F9D3E40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5EE6B9-7E6E-4923-9000-728470970A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -747,14 +747,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2366,7 +2359,7 @@
       <c r="C14" s="15">
         <v>13</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="56">
         <v>16</v>
       </c>
       <c r="E14" s="3"/>
@@ -7070,29 +7063,29 @@
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C173" s="57"/>
+      <c r="C173" s="54"/>
       <c r="D173" s="11"/>
       <c r="E173" s="10"/>
       <c r="F173" s="10"/>
       <c r="G173" s="10"/>
-      <c r="H173" s="58"/>
-      <c r="I173" s="60"/>
-      <c r="J173" s="60"/>
-      <c r="L173" s="61"/>
+      <c r="H173" s="55"/>
+      <c r="I173" s="57"/>
+      <c r="J173" s="57"/>
+      <c r="L173" s="58"/>
       <c r="M173" s="10"/>
       <c r="N173" s="10"/>
       <c r="O173" s="10"/>
       <c r="P173" s="12"/>
     </row>
     <row r="174" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C174" s="54"/>
-      <c r="F174" s="54"/>
+      <c r="C174" s="53"/>
+      <c r="F174" s="53"/>
       <c r="G174" s="11"/>
       <c r="H174" s="14"/>
-      <c r="I174" s="54"/>
+      <c r="I174" s="53"/>
       <c r="K174" s="14"/>
       <c r="L174" s="12"/>
-      <c r="P174" s="57"/>
+      <c r="P174" s="54"/>
     </row>
     <row r="175" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B175" s="21" t="s">
@@ -7175,29 +7168,29 @@
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C183" s="57"/>
+      <c r="C183" s="54"/>
       <c r="D183" s="11"/>
       <c r="E183" s="10"/>
       <c r="F183" s="10"/>
       <c r="G183" s="10"/>
-      <c r="H183" s="58"/>
-      <c r="I183" s="60"/>
-      <c r="J183" s="60"/>
-      <c r="L183" s="61"/>
+      <c r="H183" s="55"/>
+      <c r="I183" s="57"/>
+      <c r="J183" s="57"/>
+      <c r="L183" s="58"/>
       <c r="M183" s="10"/>
       <c r="N183" s="10"/>
       <c r="O183" s="10"/>
       <c r="P183" s="12"/>
     </row>
     <row r="184" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C184" s="54"/>
-      <c r="F184" s="54"/>
+      <c r="C184" s="53"/>
+      <c r="F184" s="53"/>
       <c r="G184" s="11"/>
       <c r="H184" s="14"/>
-      <c r="I184" s="54"/>
+      <c r="I184" s="53"/>
       <c r="K184" s="14"/>
       <c r="L184" s="12"/>
-      <c r="P184" s="57"/>
+      <c r="P184" s="54"/>
     </row>
     <row r="185" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B185" s="21" t="s">
@@ -7233,7 +7226,7 @@
       <c r="O185" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q185" s="55" t="s">
+      <c r="Q185" s="6" t="s">
         <v>56</v>
       </c>
       <c r="R185" s="6" t="s">
@@ -7283,30 +7276,30 @@
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C190" s="57"/>
+      <c r="C190" s="54"/>
       <c r="D190" s="11"/>
       <c r="E190" s="10"/>
       <c r="F190" s="10"/>
       <c r="G190" s="10"/>
       <c r="H190" s="10"/>
-      <c r="I190" s="58"/>
-      <c r="J190" s="60"/>
-      <c r="K190" s="60"/>
-      <c r="M190" s="61"/>
+      <c r="I190" s="55"/>
+      <c r="J190" s="57"/>
+      <c r="K190" s="57"/>
+      <c r="M190" s="58"/>
       <c r="N190" s="10"/>
       <c r="O190" s="10"/>
       <c r="P190" s="10"/>
       <c r="Q190" s="12"/>
     </row>
     <row r="191" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C191" s="54"/>
-      <c r="G191" s="54"/>
+      <c r="C191" s="53"/>
+      <c r="G191" s="53"/>
       <c r="H191" s="11"/>
       <c r="I191" s="14"/>
-      <c r="J191" s="54"/>
+      <c r="J191" s="53"/>
       <c r="L191" s="14"/>
       <c r="M191" s="12"/>
-      <c r="Q191" s="57"/>
+      <c r="Q191" s="54"/>
     </row>
     <row r="192" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B192" s="21" t="s">
@@ -7345,7 +7338,7 @@
       <c r="P192" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R192" s="55" t="s">
+      <c r="R192" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S192" s="6" t="s">
@@ -7395,30 +7388,30 @@
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C199" s="57"/>
+      <c r="C199" s="54"/>
       <c r="D199" s="11"/>
       <c r="E199" s="10"/>
       <c r="F199" s="10"/>
       <c r="G199" s="10"/>
       <c r="H199" s="10"/>
-      <c r="I199" s="58"/>
-      <c r="J199" s="60"/>
-      <c r="K199" s="60"/>
-      <c r="M199" s="61"/>
+      <c r="I199" s="55"/>
+      <c r="J199" s="57"/>
+      <c r="K199" s="57"/>
+      <c r="M199" s="58"/>
       <c r="N199" s="10"/>
       <c r="O199" s="10"/>
       <c r="P199" s="10"/>
       <c r="Q199" s="12"/>
     </row>
     <row r="200" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C200" s="54"/>
-      <c r="G200" s="54"/>
+      <c r="C200" s="53"/>
+      <c r="G200" s="53"/>
       <c r="H200" s="11"/>
       <c r="I200" s="14"/>
-      <c r="J200" s="54"/>
+      <c r="J200" s="53"/>
       <c r="L200" s="14"/>
       <c r="M200" s="12"/>
-      <c r="Q200" s="57"/>
+      <c r="Q200" s="54"/>
     </row>
     <row r="201" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B201" s="21" t="s">
@@ -7457,7 +7450,7 @@
       <c r="P201" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R201" s="55" t="s">
+      <c r="R201" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S201" s="6" t="s">
@@ -7501,7 +7494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1DF11A-C99D-4DF4-B70D-48B5B545F11B}">
   <dimension ref="A1:AL245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
       <selection activeCell="D250" sqref="D250"/>
     </sheetView>
   </sheetViews>
@@ -10068,7 +10061,7 @@
       <c r="K90" s="6">
         <v>18</v>
       </c>
-      <c r="L90" s="55">
+      <c r="L90" s="6">
         <v>21</v>
       </c>
       <c r="M90" s="3"/>
@@ -10228,10 +10221,10 @@
       <c r="K99" s="6">
         <v>18</v>
       </c>
-      <c r="L99" s="55">
+      <c r="L99" s="6">
         <v>19</v>
       </c>
-      <c r="M99" s="55">
+      <c r="M99" s="6">
         <v>21</v>
       </c>
       <c r="N99" s="3"/>
@@ -10378,10 +10371,10 @@
       <c r="L107" s="6">
         <v>18</v>
       </c>
-      <c r="M107" s="55">
+      <c r="M107" s="6">
         <v>19</v>
       </c>
-      <c r="N107" s="55">
+      <c r="N107" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10411,7 +10404,7 @@
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="33"/>
-      <c r="G115" s="62"/>
+      <c r="G115" s="59"/>
       <c r="H115" s="43"/>
       <c r="I115" s="36"/>
       <c r="J115" s="35"/>
@@ -10426,7 +10419,7 @@
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="48"/>
-      <c r="G116" s="56"/>
+      <c r="G116" s="3"/>
       <c r="H116" s="31"/>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
@@ -10449,7 +10442,7 @@
         <v>10</v>
       </c>
       <c r="F117" s="3"/>
-      <c r="G117" s="55">
+      <c r="G117" s="6">
         <v>12</v>
       </c>
       <c r="H117" s="32">
@@ -10465,10 +10458,10 @@
       <c r="L117" s="6">
         <v>18</v>
       </c>
-      <c r="M117" s="55">
+      <c r="M117" s="6">
         <v>19</v>
       </c>
-      <c r="N117" s="55">
+      <c r="N117" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10487,7 +10480,7 @@
       </c>
     </row>
     <row r="124" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F124" s="54"/>
+      <c r="F124" s="53"/>
       <c r="G124" s="52"/>
       <c r="H124" s="38"/>
       <c r="I124" s="14"/>
@@ -10516,7 +10509,7 @@
       <c r="I125" s="32">
         <v>13</v>
       </c>
-      <c r="J125" s="55">
+      <c r="J125" s="6">
         <v>14</v>
       </c>
       <c r="L125" s="6">
@@ -10528,7 +10521,7 @@
       <c r="N125" s="32">
         <v>19</v>
       </c>
-      <c r="O125" s="55">
+      <c r="O125" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10542,9 +10535,9 @@
       </c>
     </row>
     <row r="132" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E132" s="54"/>
+      <c r="E132" s="53"/>
       <c r="F132" s="11"/>
-      <c r="G132" s="58"/>
+      <c r="G132" s="55"/>
       <c r="I132" s="14"/>
       <c r="J132" s="10"/>
       <c r="K132" s="12"/>
@@ -10562,7 +10555,7 @@
       <c r="E133" s="6">
         <v>7</v>
       </c>
-      <c r="G133" s="55">
+      <c r="G133" s="6">
         <v>11</v>
       </c>
       <c r="H133" s="29">
@@ -10571,7 +10564,7 @@
       <c r="I133" s="32">
         <v>13</v>
       </c>
-      <c r="J133" s="55">
+      <c r="J133" s="6">
         <v>14</v>
       </c>
       <c r="L133" s="6">
@@ -10583,7 +10576,7 @@
       <c r="N133" s="32">
         <v>19</v>
       </c>
-      <c r="O133" s="55">
+      <c r="O133" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10602,9 +10595,9 @@
       </c>
     </row>
     <row r="139" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F139" s="54"/>
+      <c r="F139" s="53"/>
       <c r="G139" s="11"/>
-      <c r="H139" s="58"/>
+      <c r="H139" s="55"/>
       <c r="J139" s="14"/>
       <c r="K139" s="10"/>
       <c r="L139" s="12"/>
@@ -10625,7 +10618,7 @@
       <c r="F140" s="6">
         <v>7</v>
       </c>
-      <c r="H140" s="55">
+      <c r="H140" s="6">
         <v>11</v>
       </c>
       <c r="I140" s="29">
@@ -10634,7 +10627,7 @@
       <c r="J140" s="32">
         <v>13</v>
       </c>
-      <c r="K140" s="55">
+      <c r="K140" s="6">
         <v>14</v>
       </c>
       <c r="M140" s="6">
@@ -10646,7 +10639,7 @@
       <c r="O140" s="32">
         <v>19</v>
       </c>
-      <c r="P140" s="55">
+      <c r="P140" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10668,35 +10661,28 @@
       </c>
     </row>
     <row r="148" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C148" s="57"/>
+      <c r="C148" s="54"/>
       <c r="D148" s="10"/>
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
-      <c r="G148" s="61"/>
-      <c r="H148" s="65"/>
-      <c r="I148" s="58"/>
+      <c r="G148" s="58"/>
+      <c r="H148" s="62"/>
+      <c r="I148" s="55"/>
       <c r="K148" s="10"/>
       <c r="L148" s="12"/>
     </row>
     <row r="149" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C149" s="57"/>
-      <c r="F149" s="57"/>
+      <c r="C149" s="54"/>
+      <c r="F149" s="54"/>
       <c r="G149" s="10"/>
-      <c r="H149" s="53"/>
-      <c r="I149" s="57"/>
-      <c r="J149" s="53"/>
-      <c r="K149" s="53"/>
-      <c r="L149" s="57"/>
+      <c r="I149" s="54"/>
+      <c r="L149" s="54"/>
     </row>
     <row r="150" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C150" s="54"/>
-      <c r="F150" s="54"/>
-      <c r="G150" s="53"/>
-      <c r="H150" s="53"/>
-      <c r="I150" s="54"/>
-      <c r="J150" s="53"/>
-      <c r="K150" s="53"/>
-      <c r="L150" s="57"/>
+      <c r="C150" s="53"/>
+      <c r="F150" s="53"/>
+      <c r="I150" s="53"/>
+      <c r="L150" s="54"/>
     </row>
     <row r="151" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="6">
@@ -10711,7 +10697,7 @@
       <c r="F151" s="6">
         <v>7</v>
       </c>
-      <c r="H151" s="55">
+      <c r="H151" s="6">
         <v>11</v>
       </c>
       <c r="I151" s="6">
@@ -10720,7 +10706,7 @@
       <c r="J151" s="32">
         <v>13</v>
       </c>
-      <c r="K151" s="55">
+      <c r="K151" s="6">
         <v>14</v>
       </c>
       <c r="M151" s="6">
@@ -10732,7 +10718,7 @@
       <c r="O151" s="32">
         <v>19</v>
       </c>
-      <c r="P151" s="55">
+      <c r="P151" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10756,35 +10742,28 @@
       </c>
     </row>
     <row r="157" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D157" s="57"/>
+      <c r="D157" s="54"/>
       <c r="E157" s="10"/>
       <c r="F157" s="10"/>
       <c r="G157" s="10"/>
-      <c r="H157" s="61"/>
-      <c r="I157" s="65"/>
-      <c r="J157" s="58"/>
+      <c r="H157" s="58"/>
+      <c r="I157" s="62"/>
+      <c r="J157" s="55"/>
       <c r="L157" s="10"/>
       <c r="M157" s="12"/>
     </row>
     <row r="158" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D158" s="57"/>
-      <c r="G158" s="57"/>
+      <c r="D158" s="54"/>
+      <c r="G158" s="54"/>
       <c r="H158" s="10"/>
-      <c r="I158" s="53"/>
-      <c r="J158" s="57"/>
-      <c r="K158" s="53"/>
-      <c r="L158" s="53"/>
-      <c r="M158" s="57"/>
+      <c r="J158" s="54"/>
+      <c r="M158" s="54"/>
     </row>
     <row r="159" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D159" s="54"/>
-      <c r="G159" s="54"/>
-      <c r="H159" s="53"/>
-      <c r="I159" s="53"/>
-      <c r="J159" s="54"/>
-      <c r="K159" s="53"/>
-      <c r="L159" s="53"/>
-      <c r="M159" s="57"/>
+      <c r="D159" s="53"/>
+      <c r="G159" s="53"/>
+      <c r="J159" s="53"/>
+      <c r="M159" s="54"/>
     </row>
     <row r="160" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B160" s="6">
@@ -10802,7 +10781,7 @@
       <c r="G160" s="6">
         <v>7</v>
       </c>
-      <c r="I160" s="55">
+      <c r="I160" s="6">
         <v>11</v>
       </c>
       <c r="J160" s="6">
@@ -10811,7 +10790,7 @@
       <c r="K160" s="32">
         <v>13</v>
       </c>
-      <c r="L160" s="55">
+      <c r="L160" s="6">
         <v>14</v>
       </c>
       <c r="N160" s="6">
@@ -10823,7 +10802,7 @@
       <c r="P160" s="32">
         <v>19</v>
       </c>
-      <c r="Q160" s="55">
+      <c r="Q160" s="6">
         <v>21</v>
       </c>
     </row>
@@ -10846,35 +10825,28 @@
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D166" s="57"/>
+      <c r="D166" s="54"/>
       <c r="E166" s="10"/>
       <c r="F166" s="10"/>
       <c r="G166" s="10"/>
-      <c r="H166" s="61"/>
-      <c r="I166" s="65"/>
-      <c r="J166" s="58"/>
+      <c r="H166" s="58"/>
+      <c r="I166" s="62"/>
+      <c r="J166" s="55"/>
       <c r="L166" s="10"/>
       <c r="M166" s="12"/>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D167" s="57"/>
-      <c r="G167" s="57"/>
+      <c r="D167" s="54"/>
+      <c r="G167" s="54"/>
       <c r="H167" s="10"/>
-      <c r="I167" s="53"/>
-      <c r="J167" s="57"/>
-      <c r="K167" s="53"/>
-      <c r="L167" s="53"/>
-      <c r="M167" s="57"/>
+      <c r="J167" s="54"/>
+      <c r="M167" s="54"/>
     </row>
     <row r="168" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D168" s="54"/>
-      <c r="G168" s="54"/>
-      <c r="H168" s="53"/>
-      <c r="I168" s="53"/>
-      <c r="J168" s="54"/>
-      <c r="K168" s="53"/>
-      <c r="L168" s="53"/>
-      <c r="M168" s="57"/>
+      <c r="D168" s="53"/>
+      <c r="G168" s="53"/>
+      <c r="J168" s="53"/>
+      <c r="M168" s="54"/>
     </row>
     <row r="169" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B169" s="6">
@@ -10892,7 +10864,7 @@
       <c r="G169" s="6">
         <v>7</v>
       </c>
-      <c r="I169" s="55">
+      <c r="I169" s="6">
         <v>11</v>
       </c>
       <c r="J169" s="6">
@@ -10901,7 +10873,7 @@
       <c r="K169" s="32">
         <v>13</v>
       </c>
-      <c r="L169" s="55">
+      <c r="L169" s="6">
         <v>14</v>
       </c>
       <c r="N169" s="6">
@@ -10913,7 +10885,7 @@
       <c r="P169" s="32">
         <v>19</v>
       </c>
-      <c r="Q169" s="55">
+      <c r="Q169" s="6">
         <v>21</v>
       </c>
       <c r="R169" s="8">
@@ -10936,29 +10908,29 @@
       </c>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C174" s="57"/>
+      <c r="C174" s="54"/>
       <c r="D174" s="10"/>
       <c r="E174" s="10"/>
       <c r="F174" s="10"/>
-      <c r="G174" s="66"/>
-      <c r="H174" s="58"/>
-      <c r="I174" s="58"/>
-      <c r="K174" s="61"/>
-      <c r="L174" s="61"/>
+      <c r="G174" s="63"/>
+      <c r="H174" s="55"/>
+      <c r="I174" s="55"/>
+      <c r="K174" s="58"/>
+      <c r="L174" s="58"/>
       <c r="M174" s="10"/>
       <c r="N174" s="10"/>
       <c r="O174" s="12"/>
     </row>
     <row r="175" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C175" s="54"/>
-      <c r="E175" s="54"/>
+      <c r="C175" s="53"/>
+      <c r="E175" s="53"/>
       <c r="F175" s="14"/>
       <c r="G175" s="10"/>
-      <c r="H175" s="54"/>
+      <c r="H175" s="53"/>
       <c r="J175" s="14"/>
       <c r="K175" s="10"/>
       <c r="L175" s="12"/>
-      <c r="O175" s="57"/>
+      <c r="O175" s="54"/>
     </row>
     <row r="176" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="6">
@@ -10973,7 +10945,7 @@
       <c r="F176" s="6">
         <v>7</v>
       </c>
-      <c r="H176" s="55">
+      <c r="H176" s="6">
         <v>11</v>
       </c>
       <c r="I176" s="29">
@@ -10982,7 +10954,7 @@
       <c r="J176" s="32">
         <v>13</v>
       </c>
-      <c r="K176" s="55">
+      <c r="K176" s="6">
         <v>14</v>
       </c>
       <c r="M176" s="6">
@@ -10991,7 +10963,7 @@
       <c r="N176" s="6">
         <v>18</v>
       </c>
-      <c r="P176" s="55">
+      <c r="P176" s="6">
         <v>21</v>
       </c>
       <c r="Q176" s="9">
@@ -11019,29 +10991,29 @@
       </c>
     </row>
     <row r="184" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C184" s="57"/>
+      <c r="C184" s="54"/>
       <c r="D184" s="10"/>
       <c r="E184" s="10"/>
       <c r="F184" s="10"/>
-      <c r="G184" s="66"/>
-      <c r="H184" s="58"/>
-      <c r="I184" s="58"/>
-      <c r="K184" s="61"/>
-      <c r="L184" s="61"/>
+      <c r="G184" s="63"/>
+      <c r="H184" s="55"/>
+      <c r="I184" s="55"/>
+      <c r="K184" s="58"/>
+      <c r="L184" s="58"/>
       <c r="M184" s="10"/>
       <c r="N184" s="10"/>
       <c r="O184" s="12"/>
     </row>
     <row r="185" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C185" s="54"/>
-      <c r="E185" s="54"/>
+      <c r="C185" s="53"/>
+      <c r="E185" s="53"/>
       <c r="F185" s="14"/>
       <c r="G185" s="10"/>
-      <c r="H185" s="54"/>
+      <c r="H185" s="53"/>
       <c r="J185" s="14"/>
       <c r="K185" s="10"/>
       <c r="L185" s="12"/>
-      <c r="O185" s="57"/>
+      <c r="O185" s="54"/>
     </row>
     <row r="186" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B186" s="6">
@@ -11056,7 +11028,7 @@
       <c r="F186" s="6">
         <v>7</v>
       </c>
-      <c r="H186" s="55">
+      <c r="H186" s="6">
         <v>11</v>
       </c>
       <c r="I186" s="29">
@@ -11065,7 +11037,7 @@
       <c r="J186" s="32">
         <v>13</v>
       </c>
-      <c r="K186" s="55">
+      <c r="K186" s="6">
         <v>14</v>
       </c>
       <c r="M186" s="6">
@@ -11074,57 +11046,57 @@
       <c r="N186" s="6">
         <v>18</v>
       </c>
-      <c r="P186" s="55">
+      <c r="P186" s="6">
         <v>21</v>
       </c>
       <c r="Q186" s="32">
         <v>22</v>
       </c>
-      <c r="R186" s="55">
+      <c r="R186" s="6">
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="63" t="s">
+    <row r="189" spans="1:38" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B189" s="63"/>
-      <c r="C189" s="63"/>
-      <c r="D189" s="63"/>
-      <c r="E189" s="63"/>
-      <c r="F189" s="63"/>
-      <c r="G189" s="63"/>
-      <c r="H189" s="63"/>
-      <c r="I189" s="63"/>
-      <c r="J189" s="63"/>
-      <c r="K189" s="63"/>
-      <c r="L189" s="63"/>
-      <c r="M189" s="63"/>
-      <c r="N189" s="63"/>
-      <c r="O189" s="63"/>
-      <c r="P189" s="63"/>
-      <c r="Q189" s="63"/>
-      <c r="R189" s="63"/>
-      <c r="S189" s="63"/>
-      <c r="T189" s="63"/>
-      <c r="U189" s="63"/>
-      <c r="V189" s="63"/>
-      <c r="W189" s="63"/>
-      <c r="X189" s="63"/>
-      <c r="Y189" s="63"/>
-      <c r="Z189" s="63"/>
-      <c r="AA189" s="63"/>
-      <c r="AB189" s="63"/>
-      <c r="AC189" s="63"/>
-      <c r="AD189" s="63"/>
-      <c r="AE189" s="63"/>
-      <c r="AF189" s="63"/>
-      <c r="AG189" s="63"/>
-      <c r="AH189" s="63"/>
-      <c r="AI189" s="63"/>
-      <c r="AJ189" s="63"/>
-      <c r="AK189" s="63"/>
-      <c r="AL189" s="63"/>
+      <c r="B189" s="60"/>
+      <c r="C189" s="60"/>
+      <c r="D189" s="60"/>
+      <c r="E189" s="60"/>
+      <c r="F189" s="60"/>
+      <c r="G189" s="60"/>
+      <c r="H189" s="60"/>
+      <c r="I189" s="60"/>
+      <c r="J189" s="60"/>
+      <c r="K189" s="60"/>
+      <c r="L189" s="60"/>
+      <c r="M189" s="60"/>
+      <c r="N189" s="60"/>
+      <c r="O189" s="60"/>
+      <c r="P189" s="60"/>
+      <c r="Q189" s="60"/>
+      <c r="R189" s="60"/>
+      <c r="S189" s="60"/>
+      <c r="T189" s="60"/>
+      <c r="U189" s="60"/>
+      <c r="V189" s="60"/>
+      <c r="W189" s="60"/>
+      <c r="X189" s="60"/>
+      <c r="Y189" s="60"/>
+      <c r="Z189" s="60"/>
+      <c r="AA189" s="60"/>
+      <c r="AB189" s="60"/>
+      <c r="AC189" s="60"/>
+      <c r="AD189" s="60"/>
+      <c r="AE189" s="60"/>
+      <c r="AF189" s="60"/>
+      <c r="AG189" s="60"/>
+      <c r="AH189" s="60"/>
+      <c r="AI189" s="60"/>
+      <c r="AJ189" s="60"/>
+      <c r="AK189" s="60"/>
+      <c r="AL189" s="60"/>
     </row>
     <row r="190" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="191" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11142,29 +11114,29 @@
       </c>
     </row>
     <row r="192" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C192" s="57"/>
+      <c r="C192" s="54"/>
       <c r="D192" s="10"/>
       <c r="E192" s="10"/>
       <c r="F192" s="10"/>
-      <c r="G192" s="66"/>
-      <c r="H192" s="58"/>
-      <c r="I192" s="58"/>
-      <c r="K192" s="61"/>
-      <c r="L192" s="61"/>
+      <c r="G192" s="63"/>
+      <c r="H192" s="55"/>
+      <c r="I192" s="55"/>
+      <c r="K192" s="58"/>
+      <c r="L192" s="58"/>
       <c r="M192" s="10"/>
       <c r="N192" s="10"/>
       <c r="O192" s="12"/>
     </row>
     <row r="193" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C193" s="54"/>
-      <c r="E193" s="54"/>
+      <c r="C193" s="53"/>
+      <c r="E193" s="53"/>
       <c r="F193" s="14"/>
       <c r="G193" s="10"/>
-      <c r="H193" s="54"/>
+      <c r="H193" s="53"/>
       <c r="J193" s="14"/>
       <c r="K193" s="10"/>
       <c r="L193" s="12"/>
-      <c r="O193" s="57"/>
+      <c r="O193" s="54"/>
     </row>
     <row r="194" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B194" s="6">
@@ -11179,7 +11151,7 @@
       <c r="F194" s="6">
         <v>7</v>
       </c>
-      <c r="H194" s="55">
+      <c r="H194" s="6">
         <v>11</v>
       </c>
       <c r="I194" s="29">
@@ -11188,7 +11160,7 @@
       <c r="J194" s="32">
         <v>13</v>
       </c>
-      <c r="K194" s="55">
+      <c r="K194" s="6">
         <v>14</v>
       </c>
       <c r="M194" s="6">
@@ -11197,13 +11169,13 @@
       <c r="N194" s="6">
         <v>18</v>
       </c>
-      <c r="P194" s="55">
+      <c r="P194" s="6">
         <v>21</v>
       </c>
       <c r="Q194" s="32">
         <v>22</v>
       </c>
-      <c r="R194" s="55">
+      <c r="R194" s="6">
         <v>28</v>
       </c>
     </row>
@@ -11223,29 +11195,29 @@
       </c>
     </row>
     <row r="202" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C202" s="57"/>
+      <c r="C202" s="54"/>
       <c r="D202" s="10"/>
       <c r="E202" s="10"/>
       <c r="F202" s="10"/>
-      <c r="G202" s="66"/>
-      <c r="H202" s="58"/>
-      <c r="I202" s="58"/>
-      <c r="K202" s="61"/>
-      <c r="L202" s="61"/>
+      <c r="G202" s="63"/>
+      <c r="H202" s="55"/>
+      <c r="I202" s="55"/>
+      <c r="K202" s="58"/>
+      <c r="L202" s="58"/>
       <c r="M202" s="10"/>
       <c r="N202" s="10"/>
       <c r="O202" s="12"/>
     </row>
     <row r="203" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C203" s="54"/>
-      <c r="E203" s="54"/>
+      <c r="C203" s="53"/>
+      <c r="E203" s="53"/>
       <c r="F203" s="14"/>
       <c r="G203" s="10"/>
-      <c r="H203" s="54"/>
+      <c r="H203" s="53"/>
       <c r="J203" s="14"/>
       <c r="K203" s="10"/>
       <c r="L203" s="12"/>
-      <c r="O203" s="57"/>
+      <c r="O203" s="54"/>
     </row>
     <row r="204" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B204" s="6">
@@ -11260,7 +11232,7 @@
       <c r="F204" s="6">
         <v>7</v>
       </c>
-      <c r="H204" s="55">
+      <c r="H204" s="6">
         <v>11</v>
       </c>
       <c r="I204" s="29">
@@ -11269,7 +11241,7 @@
       <c r="J204" s="32">
         <v>13</v>
       </c>
-      <c r="K204" s="55">
+      <c r="K204" s="6">
         <v>14</v>
       </c>
       <c r="M204" s="6">
@@ -11281,51 +11253,51 @@
       <c r="P204" s="32">
         <v>22</v>
       </c>
-      <c r="Q204" s="55">
+      <c r="Q204" s="6">
         <v>28</v>
       </c>
     </row>
-    <row r="210" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="63" t="s">
+    <row r="210" spans="1:38" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="B210" s="63"/>
-      <c r="C210" s="63"/>
-      <c r="D210" s="63"/>
-      <c r="E210" s="63"/>
-      <c r="F210" s="63"/>
-      <c r="G210" s="63"/>
-      <c r="H210" s="63"/>
-      <c r="I210" s="63"/>
-      <c r="J210" s="63"/>
-      <c r="K210" s="63"/>
-      <c r="L210" s="63"/>
-      <c r="M210" s="63"/>
-      <c r="N210" s="63"/>
-      <c r="O210" s="63"/>
-      <c r="P210" s="63"/>
-      <c r="Q210" s="63"/>
-      <c r="R210" s="63"/>
-      <c r="S210" s="63"/>
-      <c r="T210" s="63"/>
-      <c r="U210" s="63"/>
-      <c r="V210" s="63"/>
-      <c r="W210" s="63"/>
-      <c r="X210" s="63"/>
-      <c r="Y210" s="63"/>
-      <c r="Z210" s="63"/>
-      <c r="AA210" s="63"/>
-      <c r="AB210" s="63"/>
-      <c r="AC210" s="63"/>
-      <c r="AD210" s="63"/>
-      <c r="AE210" s="63"/>
-      <c r="AF210" s="63"/>
-      <c r="AG210" s="63"/>
-      <c r="AH210" s="63"/>
-      <c r="AI210" s="63"/>
-      <c r="AJ210" s="63"/>
-      <c r="AK210" s="63"/>
-      <c r="AL210" s="63"/>
+      <c r="B210" s="60"/>
+      <c r="C210" s="60"/>
+      <c r="D210" s="60"/>
+      <c r="E210" s="60"/>
+      <c r="F210" s="60"/>
+      <c r="G210" s="60"/>
+      <c r="H210" s="60"/>
+      <c r="I210" s="60"/>
+      <c r="J210" s="60"/>
+      <c r="K210" s="60"/>
+      <c r="L210" s="60"/>
+      <c r="M210" s="60"/>
+      <c r="N210" s="60"/>
+      <c r="O210" s="60"/>
+      <c r="P210" s="60"/>
+      <c r="Q210" s="60"/>
+      <c r="R210" s="60"/>
+      <c r="S210" s="60"/>
+      <c r="T210" s="60"/>
+      <c r="U210" s="60"/>
+      <c r="V210" s="60"/>
+      <c r="W210" s="60"/>
+      <c r="X210" s="60"/>
+      <c r="Y210" s="60"/>
+      <c r="Z210" s="60"/>
+      <c r="AA210" s="60"/>
+      <c r="AB210" s="60"/>
+      <c r="AC210" s="60"/>
+      <c r="AD210" s="60"/>
+      <c r="AE210" s="60"/>
+      <c r="AF210" s="60"/>
+      <c r="AG210" s="60"/>
+      <c r="AH210" s="60"/>
+      <c r="AI210" s="60"/>
+      <c r="AJ210" s="60"/>
+      <c r="AK210" s="60"/>
+      <c r="AL210" s="60"/>
     </row>
     <row r="211" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="212" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11343,29 +11315,29 @@
       </c>
     </row>
     <row r="213" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C213" s="57"/>
+      <c r="C213" s="54"/>
       <c r="D213" s="10"/>
       <c r="E213" s="10"/>
       <c r="F213" s="10"/>
-      <c r="G213" s="66"/>
-      <c r="H213" s="58"/>
-      <c r="I213" s="58"/>
-      <c r="K213" s="61"/>
-      <c r="L213" s="61"/>
+      <c r="G213" s="63"/>
+      <c r="H213" s="55"/>
+      <c r="I213" s="55"/>
+      <c r="K213" s="58"/>
+      <c r="L213" s="58"/>
       <c r="M213" s="10"/>
       <c r="N213" s="10"/>
       <c r="O213" s="12"/>
     </row>
     <row r="214" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C214" s="54"/>
-      <c r="E214" s="54"/>
+      <c r="C214" s="53"/>
+      <c r="E214" s="53"/>
       <c r="F214" s="14"/>
       <c r="G214" s="10"/>
-      <c r="H214" s="54"/>
+      <c r="H214" s="53"/>
       <c r="J214" s="14"/>
       <c r="K214" s="10"/>
       <c r="L214" s="12"/>
-      <c r="O214" s="57"/>
+      <c r="O214" s="54"/>
     </row>
     <row r="215" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B215" s="6">
@@ -11380,7 +11352,7 @@
       <c r="F215" s="6">
         <v>7</v>
       </c>
-      <c r="H215" s="55">
+      <c r="H215" s="6">
         <v>11</v>
       </c>
       <c r="I215" s="29">
@@ -11389,7 +11361,7 @@
       <c r="J215" s="32">
         <v>13</v>
       </c>
-      <c r="K215" s="55">
+      <c r="K215" s="6">
         <v>14</v>
       </c>
       <c r="M215" s="6">
@@ -11401,7 +11373,7 @@
       <c r="P215" s="32">
         <v>22</v>
       </c>
-      <c r="Q215" s="55">
+      <c r="Q215" s="6">
         <v>28</v>
       </c>
     </row>
@@ -11421,29 +11393,29 @@
       </c>
     </row>
     <row r="222" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C222" s="57"/>
+      <c r="C222" s="54"/>
       <c r="D222" s="10"/>
       <c r="E222" s="10"/>
       <c r="F222" s="10"/>
-      <c r="G222" s="66"/>
-      <c r="H222" s="58"/>
-      <c r="I222" s="58"/>
-      <c r="K222" s="61"/>
-      <c r="L222" s="61"/>
+      <c r="G222" s="63"/>
+      <c r="H222" s="55"/>
+      <c r="I222" s="55"/>
+      <c r="K222" s="58"/>
+      <c r="L222" s="58"/>
       <c r="M222" s="10"/>
       <c r="N222" s="10"/>
       <c r="O222" s="12"/>
     </row>
     <row r="223" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C223" s="54"/>
-      <c r="E223" s="54"/>
+      <c r="C223" s="53"/>
+      <c r="E223" s="53"/>
       <c r="F223" s="14"/>
       <c r="G223" s="10"/>
-      <c r="H223" s="54"/>
+      <c r="H223" s="53"/>
       <c r="J223" s="14"/>
       <c r="K223" s="10"/>
       <c r="L223" s="12"/>
-      <c r="O223" s="57"/>
+      <c r="O223" s="54"/>
     </row>
     <row r="224" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B224" s="6">
@@ -11464,7 +11436,7 @@
       <c r="I224" s="32">
         <v>13</v>
       </c>
-      <c r="J224" s="55">
+      <c r="J224" s="6">
         <v>14</v>
       </c>
       <c r="M224" s="6">
@@ -11476,51 +11448,51 @@
       <c r="P224" s="32">
         <v>22</v>
       </c>
-      <c r="Q224" s="55">
+      <c r="Q224" s="6">
         <v>28</v>
       </c>
     </row>
-    <row r="228" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="63" t="s">
+    <row r="228" spans="1:38" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="B228" s="63"/>
-      <c r="C228" s="63"/>
-      <c r="D228" s="63"/>
-      <c r="E228" s="63"/>
-      <c r="F228" s="63"/>
-      <c r="G228" s="63"/>
-      <c r="H228" s="63"/>
-      <c r="I228" s="63"/>
-      <c r="J228" s="63"/>
-      <c r="K228" s="63"/>
-      <c r="L228" s="63"/>
-      <c r="M228" s="63"/>
-      <c r="N228" s="63"/>
-      <c r="O228" s="63"/>
-      <c r="P228" s="63"/>
-      <c r="Q228" s="63"/>
-      <c r="R228" s="63"/>
-      <c r="S228" s="63"/>
-      <c r="T228" s="63"/>
-      <c r="U228" s="63"/>
-      <c r="V228" s="63"/>
-      <c r="W228" s="63"/>
-      <c r="X228" s="63"/>
-      <c r="Y228" s="63"/>
-      <c r="Z228" s="63"/>
-      <c r="AA228" s="63"/>
-      <c r="AB228" s="63"/>
-      <c r="AC228" s="63"/>
-      <c r="AD228" s="63"/>
-      <c r="AE228" s="63"/>
-      <c r="AF228" s="63"/>
-      <c r="AG228" s="63"/>
-      <c r="AH228" s="63"/>
-      <c r="AI228" s="63"/>
-      <c r="AJ228" s="63"/>
-      <c r="AK228" s="63"/>
-      <c r="AL228" s="63"/>
+      <c r="B228" s="60"/>
+      <c r="C228" s="60"/>
+      <c r="D228" s="60"/>
+      <c r="E228" s="60"/>
+      <c r="F228" s="60"/>
+      <c r="G228" s="60"/>
+      <c r="H228" s="60"/>
+      <c r="I228" s="60"/>
+      <c r="J228" s="60"/>
+      <c r="K228" s="60"/>
+      <c r="L228" s="60"/>
+      <c r="M228" s="60"/>
+      <c r="N228" s="60"/>
+      <c r="O228" s="60"/>
+      <c r="P228" s="60"/>
+      <c r="Q228" s="60"/>
+      <c r="R228" s="60"/>
+      <c r="S228" s="60"/>
+      <c r="T228" s="60"/>
+      <c r="U228" s="60"/>
+      <c r="V228" s="60"/>
+      <c r="W228" s="60"/>
+      <c r="X228" s="60"/>
+      <c r="Y228" s="60"/>
+      <c r="Z228" s="60"/>
+      <c r="AA228" s="60"/>
+      <c r="AB228" s="60"/>
+      <c r="AC228" s="60"/>
+      <c r="AD228" s="60"/>
+      <c r="AE228" s="60"/>
+      <c r="AF228" s="60"/>
+      <c r="AG228" s="60"/>
+      <c r="AH228" s="60"/>
+      <c r="AI228" s="60"/>
+      <c r="AJ228" s="60"/>
+      <c r="AK228" s="60"/>
+      <c r="AL228" s="60"/>
     </row>
     <row r="229" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="230" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11538,29 +11510,29 @@
       </c>
     </row>
     <row r="231" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C231" s="57"/>
+      <c r="C231" s="54"/>
       <c r="D231" s="10"/>
       <c r="E231" s="10"/>
       <c r="F231" s="10"/>
-      <c r="G231" s="66"/>
-      <c r="H231" s="58"/>
-      <c r="I231" s="58"/>
-      <c r="K231" s="61"/>
-      <c r="L231" s="61"/>
+      <c r="G231" s="63"/>
+      <c r="H231" s="55"/>
+      <c r="I231" s="55"/>
+      <c r="K231" s="58"/>
+      <c r="L231" s="58"/>
       <c r="M231" s="10"/>
       <c r="N231" s="10"/>
       <c r="O231" s="12"/>
     </row>
     <row r="232" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C232" s="54"/>
-      <c r="E232" s="54"/>
+      <c r="C232" s="53"/>
+      <c r="E232" s="53"/>
       <c r="F232" s="14"/>
       <c r="G232" s="10"/>
-      <c r="H232" s="54"/>
+      <c r="H232" s="53"/>
       <c r="J232" s="14"/>
       <c r="K232" s="10"/>
       <c r="L232" s="12"/>
-      <c r="O232" s="57"/>
+      <c r="O232" s="54"/>
     </row>
     <row r="233" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B233" s="6">
@@ -11593,7 +11565,7 @@
       <c r="P233" s="32">
         <v>22</v>
       </c>
-      <c r="Q233" s="55">
+      <c r="Q233" s="6">
         <v>28</v>
       </c>
     </row>
@@ -11613,29 +11585,29 @@
       </c>
     </row>
     <row r="240" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C240" s="57"/>
+      <c r="C240" s="54"/>
       <c r="D240" s="10"/>
       <c r="E240" s="10"/>
       <c r="F240" s="10"/>
-      <c r="G240" s="66"/>
-      <c r="H240" s="58"/>
-      <c r="I240" s="58"/>
-      <c r="K240" s="61"/>
-      <c r="L240" s="61"/>
+      <c r="G240" s="63"/>
+      <c r="H240" s="55"/>
+      <c r="I240" s="55"/>
+      <c r="K240" s="58"/>
+      <c r="L240" s="58"/>
       <c r="M240" s="10"/>
       <c r="N240" s="10"/>
       <c r="O240" s="12"/>
     </row>
     <row r="241" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C241" s="54"/>
-      <c r="E241" s="54"/>
+      <c r="C241" s="53"/>
+      <c r="E241" s="53"/>
       <c r="F241" s="14"/>
       <c r="G241" s="10"/>
-      <c r="H241" s="54"/>
+      <c r="H241" s="53"/>
       <c r="J241" s="10"/>
       <c r="K241" s="10"/>
       <c r="L241" s="12"/>
-      <c r="O241" s="57"/>
+      <c r="O241" s="54"/>
     </row>
     <row r="242" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B242" s="6">
@@ -11656,7 +11628,6 @@
       <c r="I242" s="32">
         <v>13</v>
       </c>
-      <c r="J242" s="53"/>
       <c r="L242" s="6">
         <v>16</v>
       </c>
@@ -11666,7 +11637,7 @@
       <c r="O242" s="32">
         <v>22</v>
       </c>
-      <c r="P242" s="55">
+      <c r="P242" s="6">
         <v>28</v>
       </c>
     </row>

</xml_diff>